<commit_message>
add log format process
</commit_message>
<xml_diff>
--- a/config/counter_define.xlsx
+++ b/config/counter_define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Counter定义" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>IE名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,10 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>equal</t>
   </si>
   <si>
@@ -119,7 +115,17 @@
     <t>section</t>
   </si>
   <si>
+    <t>avg</t>
+  </si>
+  <si>
     <t>range</t>
+  </si>
+  <si>
+    <t>106-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,8 +252,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -277,20 +309,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,8 +334,20 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -318,6 +362,9 @@
     <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +379,9 @@
     <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,15 +713,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
@@ -680,69 +730,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="44" customHeight="1">
@@ -750,18 +800,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="3">
+        <v>100</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -775,14 +829,14 @@
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -800,14 +854,14 @@
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -823,13 +877,23 @@
     <row r="6" spans="1:15">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -840,8 +904,8 @@
     <row r="7" spans="1:15">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -857,8 +921,8 @@
     <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="3"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -874,8 +938,8 @@
     <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -891,8 +955,8 @@
     <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -908,8 +972,8 @@
     <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="3"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -925,8 +989,8 @@
     <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -942,8 +1006,8 @@
     <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -959,8 +1023,8 @@
     <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -976,8 +1040,8 @@
     <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -993,8 +1057,8 @@
     <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1010,8 +1074,8 @@
     <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1027,8 +1091,8 @@
     <row r="18" spans="1:15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1044,8 +1108,8 @@
     <row r="19" spans="1:15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1061,8 +1125,8 @@
     <row r="20" spans="1:15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1078,8 +1142,8 @@
     <row r="21" spans="1:15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1095,8 +1159,8 @@
     <row r="22" spans="1:15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1112,8 +1176,8 @@
     <row r="23" spans="1:15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1129,8 +1193,8 @@
     <row r="24" spans="1:15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1146,8 +1210,8 @@
     <row r="25" spans="1:15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1163,8 +1227,8 @@
     <row r="26" spans="1:15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1180,8 +1244,8 @@
     <row r="27" spans="1:15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1197,8 +1261,8 @@
     <row r="28" spans="1:15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="1"/>
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1216,17 +1280,17 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:O1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N28 K3:K28 H3:H28 E3:E28">
       <formula1>"range,section,equal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C28">
       <formula1>"max,min,avg,recent"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1245,7 +1309,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add merge lgl file function
</commit_message>
<xml_diff>
--- a/config/counter_define.xlsx
+++ b/config/counter_define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="1760" windowWidth="24720" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Counter定义" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
report value code refactor
</commit_message>
<xml_diff>
--- a/config/counter_define.xlsx
+++ b/config/counter_define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1760" windowWidth="24720" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24160" windowHeight="15060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Counter定义" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,6 +246,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -280,7 +306,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -302,6 +328,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -668,7 +700,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -690,7 +722,7 @@
       <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -714,10 +746,10 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>

</xml_diff>

<commit_message>
add report process function
</commit_message>
<xml_diff>
--- a/config/counter_define.xlsx
+++ b/config/counter_define.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24160" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="12120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Counter定义" sheetId="1" r:id="rId1"/>
     <sheet name="KPI定义" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>IE名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,85 +42,108 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>FTP_RSRP_Min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FTP_RSRP_Avg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联IE 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关系 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关系 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联IE 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关系 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联IE 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>FTP_RSRP_Max</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FTP_RSRP_Min</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FTP_RSRP_Avg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
-  </si>
-  <si>
-    <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TDDLTE_L1_measurement_Serving_Cell_Measurement_RSRP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FTP_RSRP_Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>[-75,-72]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-72,-72]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>equal</t>
-  </si>
-  <si>
-    <t>范围</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关联条件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关联IE 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>范围 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关系 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>范围 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关系 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关联IE 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>范围 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关系 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关联IE 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -172,6 +195,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -273,7 +297,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,8 +329,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,17 +353,25 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -353,25 +387,99 @@
     <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -383,7 +491,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -700,103 +808,105 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" customWidth="1"/>
+    <col min="11" max="11" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1">
+        <v>9</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="44.1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="44" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -806,21 +916,23 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="54" customHeight="1">
+    <row r="4" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -831,21 +943,19 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="56" customHeight="1">
+    <row r="5" spans="1:15" ht="56.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -856,13 +966,23 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="12">
+        <v>-71</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -873,13 +993,13 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -890,13 +1010,13 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
@@ -907,13 +1027,13 @@
       <c r="N8" s="3"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
@@ -924,13 +1044,13 @@
       <c r="N9" s="3"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
@@ -941,13 +1061,13 @@
       <c r="N10" s="3"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="1"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
@@ -958,13 +1078,13 @@
       <c r="N11" s="3"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="1"/>
       <c r="H12" s="3"/>
       <c r="I12" s="1"/>
@@ -975,13 +1095,13 @@
       <c r="N12" s="3"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="1"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1"/>
@@ -992,13 +1112,13 @@
       <c r="N13" s="3"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="1"/>
       <c r="H14" s="3"/>
       <c r="I14" s="1"/>
@@ -1009,13 +1129,13 @@
       <c r="N14" s="3"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="1"/>
@@ -1026,13 +1146,13 @@
       <c r="N15" s="3"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="1"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
@@ -1043,13 +1163,13 @@
       <c r="N16" s="3"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
@@ -1060,13 +1180,13 @@
       <c r="N17" s="3"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="1"/>
       <c r="H18" s="3"/>
       <c r="I18" s="1"/>
@@ -1077,13 +1197,13 @@
       <c r="N18" s="3"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="3"/>
       <c r="I19" s="1"/>
@@ -1094,13 +1214,13 @@
       <c r="N19" s="3"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="1"/>
       <c r="H20" s="3"/>
       <c r="I20" s="1"/>
@@ -1111,13 +1231,13 @@
       <c r="N20" s="3"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="1"/>
       <c r="H21" s="3"/>
       <c r="I21" s="1"/>
@@ -1128,13 +1248,13 @@
       <c r="N21" s="3"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="1"/>
       <c r="H22" s="3"/>
       <c r="I22" s="1"/>
@@ -1145,13 +1265,13 @@
       <c r="N22" s="3"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="1"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
@@ -1162,13 +1282,13 @@
       <c r="N23" s="3"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
@@ -1179,13 +1299,13 @@
       <c r="N24" s="3"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="1"/>
       <c r="H25" s="3"/>
       <c r="I25" s="1"/>
@@ -1196,13 +1316,13 @@
       <c r="N25" s="3"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="1"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
@@ -1213,13 +1333,13 @@
       <c r="N26" s="3"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1"/>
       <c r="H27" s="3"/>
       <c r="I27" s="1"/>
@@ -1230,13 +1350,13 @@
       <c r="N27" s="3"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="1"/>
       <c r="H28" s="3"/>
       <c r="I28" s="1"/>
@@ -1258,16 +1378,19 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N28 K3:K28 H3:H28 E3:E28">
       <formula1>"range,section,equal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C28">
       <formula1>"max,min,avg,recent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6">
+      <formula1>"max,min,avg,recent,count"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1284,7 +1407,7 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add section and array function
</commit_message>
<xml_diff>
--- a/config/counter_define.xlsx
+++ b/config/counter_define.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>IE名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,24 +126,6 @@
   </si>
   <si>
     <t>avg</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>[-75,-72]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[-72,-72]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>equal</t>
   </si>
 </sst>
 </file>
@@ -350,6 +332,13 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -362,13 +351,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -805,15 +787,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
@@ -824,43 +806,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
@@ -900,15 +882,11 @@
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -927,16 +905,12 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -955,8 +929,8 @@
         <v>8</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -977,12 +951,8 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="12">
-        <v>-71</v>
-      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -999,7 +969,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1016,7 +986,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
@@ -1033,7 +1003,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
@@ -1050,7 +1020,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
@@ -1067,7 +1037,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="1"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
@@ -1084,7 +1054,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="1"/>
       <c r="H12" s="3"/>
       <c r="I12" s="1"/>
@@ -1101,7 +1071,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="1"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1"/>
@@ -1118,7 +1088,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="1"/>
       <c r="H14" s="3"/>
       <c r="I14" s="1"/>
@@ -1135,7 +1105,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="13"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="1"/>
@@ -1152,7 +1122,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="1"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
@@ -1169,7 +1139,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
@@ -1186,7 +1156,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="1"/>
       <c r="H18" s="3"/>
       <c r="I18" s="1"/>
@@ -1203,7 +1173,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="13"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="1"/>
       <c r="H19" s="3"/>
       <c r="I19" s="1"/>
@@ -1220,7 +1190,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="13"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="1"/>
       <c r="H20" s="3"/>
       <c r="I20" s="1"/>
@@ -1237,7 +1207,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="13"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="1"/>
       <c r="H21" s="3"/>
       <c r="I21" s="1"/>
@@ -1254,7 +1224,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="13"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="1"/>
       <c r="H22" s="3"/>
       <c r="I22" s="1"/>
@@ -1271,7 +1241,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="1"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
@@ -1288,7 +1258,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="13"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
@@ -1305,7 +1275,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="13"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="1"/>
       <c r="H25" s="3"/>
       <c r="I25" s="1"/>
@@ -1322,7 +1292,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="13"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="1"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
@@ -1332,40 +1302,6 @@
       <c r="M26" s="1"/>
       <c r="N26" s="3"/>
       <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1378,15 +1314,18 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N28 K3:K28 H3:H28 E3:E28">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K26 N3:N26 H3:H26">
       <formula1>"range,section,equal"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C28">
-      <formula1>"max,min,avg,recent"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6">
       <formula1>"max,min,avg,recent,count"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C26">
+      <formula1>"max,min,avg,recent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E26">
+      <formula1>"range,section,equal,array"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>